<commit_message>
Refactor gold and stock data fetching: move logic to Stock_market.py, remove gold.py, and add API reference documentation
</commit_message>
<xml_diff>
--- a/market_data.xlsx
+++ b/market_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,42 @@
         <v>21213.97</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-12-31 21:00:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-01-01 02:30:00</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>250.42</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20784.86</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-147.74</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.71</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21022.24</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20702.69</v>
+      </c>
+      <c r="I4" t="n">
+        <v>20952.52</v>
+      </c>
+      <c r="J4" t="n">
+        <v>20932.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add API reference documentation and create Excel file for FAANG stock APIs
</commit_message>
<xml_diff>
--- a/market_data.xlsx
+++ b/market_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Apple Stock" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Gold Prices" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +594,131 @@
         <v>20932.6</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-12-31 21:00:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-01-01 02:30:00</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>250.42</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20784.86</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-147.74</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.71</v>
+      </c>
+      <c r="G5" t="n">
+        <v>21022.24</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20702.69</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20952.52</v>
+      </c>
+      <c r="J5" t="n">
+        <v>20932.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>24K Price (INR/g)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>22K Price (INR/g)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>18K Price (INR/g)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-01-01 05:17:26</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>7230.6965</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6628.1384</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5423.0224</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-01-01 06:57:12</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7232.3844</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6629.6857</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5424.2883</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-01-01 06:57:12</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7232.3844</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6629.6857</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5424.2883</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>